<commit_message>
adicionei tau2 nas figuras desubgrupos
</commit_message>
<xml_diff>
--- a/data/subgruposppt.xlsx
+++ b/data/subgruposppt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufscbr-my.sharepoint.com/personal/tamires_martins_ufsc_br/Documents/PC LAB/DissAnalysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_AD4D361C20488DEA4E38A055DC1A575E5BDEDD85" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16F47286-8317-412C-B128-F0DD5E5F97E2}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="11_AD4D361C20488DEA4E38A055DC1A575E5BDEDD85" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{463B93B6-92FA-444A-943A-7D1D14B2D924}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="124">
   <si>
     <t>Sexo</t>
   </si>
@@ -444,6 +444,9 @@
   </si>
   <si>
     <t>Revista revisada por pares</t>
+  </si>
+  <si>
+    <t>tau2</t>
   </si>
 </sst>
 </file>
@@ -822,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J134"/>
+  <dimension ref="A1:K134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="K122" sqref="K122"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,7 +846,7 @@
     <col min="11" max="16384" width="15.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>41</v>
       </c>
@@ -874,8 +877,11 @@
       <c r="J1" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>42</v>
       </c>
@@ -906,8 +912,11 @@
       <c r="J2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="1">
+        <v>2.0699999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
@@ -938,8 +947,11 @@
       <c r="J3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="1">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
@@ -970,8 +982,11 @@
       <c r="J4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
@@ -1002,8 +1017,11 @@
       <c r="J5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" s="1">
+        <v>3.71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>42</v>
       </c>
@@ -1034,8 +1052,11 @@
       <c r="J6" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="1">
+        <v>33.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
@@ -1066,8 +1087,11 @@
       <c r="J7" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" s="1">
+        <v>6.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
@@ -1098,8 +1122,11 @@
       <c r="J8" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="1">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
@@ -1130,8 +1157,11 @@
       <c r="J9" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="1">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>42</v>
       </c>
@@ -1162,8 +1192,11 @@
       <c r="J10" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>42</v>
       </c>
@@ -1194,8 +1227,11 @@
       <c r="J11" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="1">
+        <v>77.52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
@@ -1226,8 +1262,11 @@
       <c r="J12" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="1">
+        <v>12.37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
@@ -1258,8 +1297,11 @@
       <c r="J13" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" s="1">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
@@ -1290,8 +1332,11 @@
       <c r="J14" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="1">
+        <v>2.41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
@@ -1322,8 +1367,11 @@
       <c r="J15" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>42</v>
       </c>
@@ -1354,8 +1402,11 @@
       <c r="J16" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="1">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
@@ -1386,8 +1437,11 @@
       <c r="J17" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="1">
+        <v>15.72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>42</v>
       </c>
@@ -1418,8 +1472,11 @@
       <c r="J18" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>42</v>
       </c>
@@ -1450,8 +1507,11 @@
       <c r="J19" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="1">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>42</v>
       </c>
@@ -1482,8 +1542,11 @@
       <c r="J20" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>42</v>
       </c>
@@ -1514,8 +1577,11 @@
       <c r="J21" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="1">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -1546,8 +1612,11 @@
       <c r="J22" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="1">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -1578,8 +1647,11 @@
       <c r="J23" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="1">
+        <v>3.55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
@@ -1610,8 +1682,11 @@
       <c r="J24" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="1">
+        <v>68.11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>42</v>
       </c>
@@ -1642,8 +1717,11 @@
       <c r="J25" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="1">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>42</v>
       </c>
@@ -1674,8 +1752,11 @@
       <c r="J26" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" s="1">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>42</v>
       </c>
@@ -1706,8 +1787,11 @@
       <c r="J27" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" s="1">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>42</v>
       </c>
@@ -1738,8 +1822,11 @@
       <c r="J28" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" s="1">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>42</v>
       </c>
@@ -1770,8 +1857,11 @@
       <c r="J29" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" s="1">
+        <v>64.7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>42</v>
       </c>
@@ -1802,8 +1892,11 @@
       <c r="J30" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" s="1">
+        <v>2.65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>42</v>
       </c>
@@ -1834,8 +1927,11 @@
       <c r="J31" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" s="1">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>42</v>
       </c>
@@ -1866,8 +1962,11 @@
       <c r="J32" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" s="1">
+        <v>7.84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>42</v>
       </c>
@@ -1898,8 +1997,11 @@
       <c r="J33" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" s="1">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>42</v>
       </c>
@@ -1930,8 +2032,11 @@
       <c r="J34" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34" s="1">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
@@ -1962,8 +2067,11 @@
       <c r="J35" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35" s="1">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -1994,8 +2102,11 @@
       <c r="J36" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36" s="1">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>42</v>
       </c>
@@ -2026,8 +2137,11 @@
       <c r="J37" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37" s="1">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>42</v>
       </c>
@@ -2058,8 +2172,11 @@
       <c r="J38" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38" s="1">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>42</v>
       </c>
@@ -2090,8 +2207,11 @@
       <c r="J39" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39" s="1">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>
@@ -2122,8 +2242,11 @@
       <c r="J40" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K40" s="1">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
@@ -2154,8 +2277,11 @@
       <c r="J41" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41" s="1">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
@@ -2186,8 +2312,11 @@
       <c r="J42" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K42" s="1">
+        <v>18.440000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
@@ -2218,8 +2347,11 @@
       <c r="J43" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K43" s="1">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -2250,8 +2382,11 @@
       <c r="J44" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K44" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
@@ -2282,8 +2417,11 @@
       <c r="J45" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45" s="1">
+        <v>1.37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>54</v>
       </c>
@@ -2314,8 +2452,11 @@
       <c r="J46" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K46" s="1">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>54</v>
       </c>
@@ -2346,8 +2487,11 @@
       <c r="J47" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K47" s="1">
+        <v>14.22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>54</v>
       </c>
@@ -2378,8 +2522,11 @@
       <c r="J48" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K48" s="1">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
@@ -2410,8 +2557,11 @@
       <c r="J49" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K49" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>54</v>
       </c>
@@ -2442,8 +2592,11 @@
       <c r="J50" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K50" s="1">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>54</v>
       </c>
@@ -2474,8 +2627,11 @@
       <c r="J51" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K51" s="1">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>54</v>
       </c>
@@ -2506,8 +2662,11 @@
       <c r="J52" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K52" s="1">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>54</v>
       </c>
@@ -2538,8 +2697,11 @@
       <c r="J53" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K53" s="1">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>54</v>
       </c>
@@ -2570,8 +2732,11 @@
       <c r="J54" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>54</v>
       </c>
@@ -2602,8 +2767,11 @@
       <c r="J55" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K55" s="1">
+        <v>16.72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
@@ -2634,8 +2802,11 @@
       <c r="J56" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K56" s="1">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>54</v>
       </c>
@@ -2666,8 +2837,11 @@
       <c r="J57" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K57" s="1">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>54</v>
       </c>
@@ -2698,8 +2872,11 @@
       <c r="J58" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K58" s="1">
+        <v>3.64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>54</v>
       </c>
@@ -2730,8 +2907,11 @@
       <c r="J59" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K59" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>54</v>
       </c>
@@ -2762,8 +2942,11 @@
       <c r="J60" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K60" s="1">
+        <v>21.92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>54</v>
       </c>
@@ -2794,8 +2977,11 @@
       <c r="J61" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K61" s="1">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>54</v>
       </c>
@@ -2826,8 +3012,11 @@
       <c r="J62" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K62" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>54</v>
       </c>
@@ -2858,8 +3047,11 @@
       <c r="J63" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K63" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>54</v>
       </c>
@@ -2890,8 +3082,11 @@
       <c r="J64" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K64" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>54</v>
       </c>
@@ -2922,8 +3117,11 @@
       <c r="J65" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K65" s="1">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>54</v>
       </c>
@@ -2954,8 +3152,11 @@
       <c r="J66" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K66" s="1">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>54</v>
       </c>
@@ -2986,8 +3187,11 @@
       <c r="J67" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K67" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>54</v>
       </c>
@@ -3018,8 +3222,11 @@
       <c r="J68" s="9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K68" s="1">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>54</v>
       </c>
@@ -3050,8 +3257,11 @@
       <c r="J69" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K69" s="1">
+        <v>3.32</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>54</v>
       </c>
@@ -3082,8 +3292,11 @@
       <c r="J70" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K70" s="1">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>54</v>
       </c>
@@ -3114,8 +3327,11 @@
       <c r="J71" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K71" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>54</v>
       </c>
@@ -3146,8 +3362,11 @@
       <c r="J72" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K72" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>54</v>
       </c>
@@ -3178,8 +3397,11 @@
       <c r="J73" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K73" s="1">
+        <v>1.98</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>54</v>
       </c>
@@ -3210,8 +3432,11 @@
       <c r="J74" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K74" s="1">
+        <v>6.88</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>54</v>
       </c>
@@ -3242,8 +3467,11 @@
       <c r="J75" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K75" s="1">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>54</v>
       </c>
@@ -3274,8 +3502,11 @@
       <c r="J76" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K76" s="1">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>54</v>
       </c>
@@ -3306,8 +3537,11 @@
       <c r="J77" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K77" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>54</v>
       </c>
@@ -3338,8 +3572,11 @@
       <c r="J78" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K78" s="1">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>54</v>
       </c>
@@ -3370,8 +3607,11 @@
       <c r="J79" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K79" s="1">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>54</v>
       </c>
@@ -3402,8 +3642,11 @@
       <c r="J80" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K80" s="1">
+        <v>2.46</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>54</v>
       </c>
@@ -3434,8 +3677,11 @@
       <c r="J81" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K81" s="1">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>54</v>
       </c>
@@ -3466,8 +3712,11 @@
       <c r="J82" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K82" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>54</v>
       </c>
@@ -3498,8 +3747,11 @@
       <c r="J83" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K83" s="1">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>54</v>
       </c>
@@ -3530,8 +3782,11 @@
       <c r="J84" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K84" s="1">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>54</v>
       </c>
@@ -3562,8 +3817,11 @@
       <c r="J85" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K85" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>54</v>
       </c>
@@ -3594,8 +3852,11 @@
       <c r="J86" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K86" s="1">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>54</v>
       </c>
@@ -3626,8 +3887,11 @@
       <c r="J87" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K87" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>54</v>
       </c>
@@ -3658,8 +3922,11 @@
       <c r="J88" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K88" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>54</v>
       </c>
@@ -3690,8 +3957,11 @@
       <c r="J89" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K89" s="1">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>54</v>
       </c>
@@ -3722,8 +3992,11 @@
       <c r="J90" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K90" s="1">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>54</v>
       </c>
@@ -3754,8 +4027,11 @@
       <c r="J91" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K91" s="1">
+        <v>2.64</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>54</v>
       </c>
@@ -3786,8 +4062,11 @@
       <c r="J92" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K92" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>54</v>
       </c>
@@ -3818,8 +4097,11 @@
       <c r="J93" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K93" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>54</v>
       </c>
@@ -3850,8 +4132,11 @@
       <c r="J94" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K94" s="1">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>54</v>
       </c>
@@ -3882,8 +4167,11 @@
       <c r="J95" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K95" s="1">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>54</v>
       </c>
@@ -3914,8 +4202,11 @@
       <c r="J96" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K96" s="1">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>54</v>
       </c>
@@ -3946,8 +4237,11 @@
       <c r="J97" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K97" s="1">
+        <v>32.61</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>54</v>
       </c>
@@ -3978,8 +4272,11 @@
       <c r="J98" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K98" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>54</v>
       </c>
@@ -4010,8 +4307,11 @@
       <c r="J99" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K99" s="1">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>54</v>
       </c>
@@ -4042,8 +4342,11 @@
       <c r="J100" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="101" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K100" s="1">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>95</v>
       </c>
@@ -4074,8 +4377,11 @@
       <c r="J101" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="102" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K101" s="1">
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>95</v>
       </c>
@@ -4106,8 +4412,11 @@
       <c r="J102" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="103" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K102" s="1">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>95</v>
       </c>
@@ -4138,8 +4447,11 @@
       <c r="J103" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="104" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K103" s="1">
+        <v>20.76</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>95</v>
       </c>
@@ -4170,8 +4482,11 @@
       <c r="J104" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="105" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K104" s="1">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>95</v>
       </c>
@@ -4202,8 +4517,11 @@
       <c r="J105" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="106" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K105" s="1">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>95</v>
       </c>
@@ -4234,8 +4552,11 @@
       <c r="J106" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="107" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K106" s="1">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>95</v>
       </c>
@@ -4266,8 +4587,11 @@
       <c r="J107" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="108" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K107" s="1">
+        <v>69.25</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>95</v>
       </c>
@@ -4298,8 +4622,11 @@
       <c r="J108" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="109" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K108" s="1">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>95</v>
       </c>
@@ -4330,8 +4657,11 @@
       <c r="J109" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="110" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K109" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>95</v>
       </c>
@@ -4362,8 +4692,11 @@
       <c r="J110" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="111" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K110" s="1">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>95</v>
       </c>
@@ -4394,8 +4727,11 @@
       <c r="J111" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="112" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K111" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>95</v>
       </c>
@@ -4426,8 +4762,11 @@
       <c r="J112" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K112" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>95</v>
       </c>
@@ -4458,8 +4797,11 @@
       <c r="J113" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K113" s="1">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>95</v>
       </c>
@@ -4490,8 +4832,11 @@
       <c r="J114" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K114" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>95</v>
       </c>
@@ -4522,8 +4867,11 @@
       <c r="J115" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K115" s="1">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>95</v>
       </c>
@@ -4554,8 +4902,11 @@
       <c r="J116" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K116" s="1">
+        <v>3.51</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>95</v>
       </c>
@@ -4586,8 +4937,11 @@
       <c r="J117" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K117" s="1">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>95</v>
       </c>
@@ -4618,8 +4972,11 @@
       <c r="J118" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K118" s="1">
+        <v>7.52</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>95</v>
       </c>
@@ -4650,8 +5007,11 @@
       <c r="J119" s="9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K119" s="1">
+        <v>2.19</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>95</v>
       </c>
@@ -4682,8 +5042,11 @@
       <c r="J120" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K120" s="1">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>95</v>
       </c>
@@ -4714,8 +5077,11 @@
       <c r="J121" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="K121" s="1">
+        <v>38.130000000000003</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>95</v>
       </c>
@@ -4746,8 +5112,11 @@
       <c r="J122" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K122" s="1">
+        <v>1.87</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>95</v>
       </c>
@@ -4778,8 +5147,11 @@
       <c r="J123" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K123" s="1">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>95</v>
       </c>
@@ -4810,8 +5182,11 @@
       <c r="J124" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K124" s="1">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>95</v>
       </c>
@@ -4842,8 +5217,11 @@
       <c r="J125" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K125" s="1">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>95</v>
       </c>
@@ -4874,8 +5252,11 @@
       <c r="J126" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K126" s="1">
+        <v>5.0599999999999996</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>95</v>
       </c>
@@ -4906,8 +5287,11 @@
       <c r="J127" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K127" s="1">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>95</v>
       </c>
@@ -4938,8 +5322,11 @@
       <c r="J128" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="129" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="K128" s="1">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>95</v>
       </c>
@@ -4970,8 +5357,11 @@
       <c r="J129" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K129" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>95</v>
       </c>
@@ -5002,8 +5392,11 @@
       <c r="J130" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K130" s="1">
+        <v>3.46</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>95</v>
       </c>
@@ -5034,8 +5427,11 @@
       <c r="J131" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K131" s="1">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>95</v>
       </c>
@@ -5066,8 +5462,11 @@
       <c r="J132" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K132" s="1">
+        <v>2.31</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>95</v>
       </c>
@@ -5098,8 +5497,11 @@
       <c r="J133" s="9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K133" s="1">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>95</v>
       </c>
@@ -5129,6 +5531,9 @@
       </c>
       <c r="J134" s="9" t="s">
         <v>4</v>
+      </c>
+      <c r="K134" s="1">
+        <v>1.64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>